<commit_message>
updates to distribution fittings
</commit_message>
<xml_diff>
--- a/Example_Spreadsheet_v072622.xlsx
+++ b/Example_Spreadsheet_v072622.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="14" documentId="8_{02B1327D-6B4E-4E29-939B-7F05390488CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE90FD9A-4B85-4185-BBB4-49B04B41BCA4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7485" yWindow="4965" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow Scenarios" sheetId="1" r:id="rId1"/>
@@ -536,10 +536,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1413,7 +1413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:HA16"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:R9"/>
     </sheetView>
   </sheetViews>
@@ -1461,165 +1461,165 @@
       <c r="S1" s="12"/>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
       <c r="S2" s="13"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
       <c r="S3" s="13"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
       <c r="S7" s="19"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
       <c r="S8" s="13"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
       <c r="S9" s="13"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -1655,8 +1655,8 @@
       <c r="F11" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="35"/>
       <c r="J11" s="35"/>
       <c r="K11" s="35"/>
@@ -1667,8 +1667,8 @@
       <c r="P11" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
       <c r="S11" s="14"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -1925,7 +1925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AU1745"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -1951,73 +1951,73 @@
       <c r="B2" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -14284,57 +14284,57 @@
       <c r="B2" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
@@ -25305,7 +25305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -25346,41 +25346,41 @@
       <c r="B2" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
     </row>
     <row r="3" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
     </row>
     <row r="4" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>

</xml_diff>